<commit_message>
Agrega ejecucion parcial con BE y BL
</commit_message>
<xml_diff>
--- a/data/Resultados_AG.xlsx
+++ b/data/Resultados_AG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasal\Google Drive\EAFIT\Ciencia de Datos y Analitica\03 Tercer Semestre\Metodos Heuristicos para Optimizacion\metodos-heuristicos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C290B30-97A0-47CD-8827-F990199678D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7860BD67-FAC4-4E54-BEC1-09B8F2DEC368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B1250CC-1120-467C-8907-0AF514310821}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B1250CC-1120-467C-8907-0AF514310821}"/>
   </bookViews>
   <sheets>
     <sheet name="AG" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="39">
   <si>
     <t>Precision</t>
   </si>
@@ -102,14 +102,63 @@
   </si>
   <si>
     <t>(peor solucion)</t>
+  </si>
+  <si>
+    <t>INTENSIFICACION</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Precision-AUC</t>
+  </si>
+  <si>
+    <t>Recall-AUC</t>
+  </si>
+  <si>
+    <t>FScore-AUC</t>
+  </si>
+  <si>
+    <t>LS-RB1</t>
+  </si>
+  <si>
+    <t>RB2-V25</t>
+  </si>
+  <si>
+    <t>RB2-V64</t>
+  </si>
+  <si>
+    <t>SEL</t>
+  </si>
+  <si>
+    <t>Fscore</t>
+  </si>
+  <si>
+    <t>Función de Activación</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Identity</t>
+  </si>
+  <si>
+    <t>Logistic</t>
+  </si>
+  <si>
+    <t>Relu</t>
+  </si>
+  <si>
+    <t>Tanh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -358,7 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -407,6 +456,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -419,41 +513,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,6 +557,931 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.0851226639912743E-2"/>
+          <c:y val="4.9717514124293788E-2"/>
+          <c:w val="0.93829754672017451"/>
+          <c:h val="0.83632439165443306"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AG!$P$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-E49F-4889-9EC9-98927150332E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-E49F-4889-9EC9-98927150332E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>AG!$O$31:$O$34</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Identity</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Relu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tanh</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Logistic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AG!$P$31:$P$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.88500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E49F-4889-9EC9-98927150332E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="59"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1261586448"/>
+        <c:axId val="1255648832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1261586448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="28575" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1255648832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1255648832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.93"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1261586448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>664847</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>78105</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>453390</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB26B758-E3E8-4BA2-AF85-2908C3E08911}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -769,10 +1781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0DA66-6DF4-4FA4-8913-44EB5171D2D4}">
-  <dimension ref="D2:S58"/>
+  <dimension ref="D2:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="G28" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,25 +1802,25 @@
   <sheetData>
     <row r="2" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="24" t="s">
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="26"/>
-      <c r="O3" s="24" t="s">
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="49"/>
+      <c r="O3" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="26"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="49"/>
     </row>
     <row r="4" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
@@ -859,7 +1871,7 @@
         <f>+(E5-Q5)/Q5</f>
         <v>-1.8293715981854121E-2</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="28">
         <v>6.2713999304782497E-2</v>
       </c>
       <c r="H5" s="19">
@@ -873,7 +1885,7 @@
         <f>(I5-Q5)/Q5</f>
         <v>-1.100243998455078E-2</v>
       </c>
-      <c r="K5" s="39">
+      <c r="K5" s="28">
         <v>6.3378184036520596E-2</v>
       </c>
       <c r="L5" s="19">
@@ -903,7 +1915,7 @@
         <f>+(E6-Q6)/Q6</f>
         <v>1.7555187933877524E-3</v>
       </c>
-      <c r="G6" s="39">
+      <c r="G6" s="28">
         <v>0.77462296258586505</v>
       </c>
       <c r="H6" s="19">
@@ -917,7 +1929,7 @@
         <f>(I6-Q6)/Q6</f>
         <v>-1.2043473760078916E-4</v>
       </c>
-      <c r="K6" s="39">
+      <c r="K6" s="28">
         <v>0.77282431393572204</v>
       </c>
       <c r="L6" s="19">
@@ -947,7 +1959,7 @@
         <f>+(E7-Q7)/Q7</f>
         <v>4.6800181748277242E-2</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="28">
         <v>7.1068371056643598E-2</v>
       </c>
       <c r="H7" s="19">
@@ -961,7 +1973,7 @@
         <f>(I7-Q7)/Q7</f>
         <v>-3.7377188637693903E-2</v>
       </c>
-      <c r="K7" s="39">
+      <c r="K7" s="28">
         <v>6.5474527335382296E-2</v>
       </c>
       <c r="L7" s="19">
@@ -991,7 +2003,7 @@
         <f>+(E8-Q8)/Q8</f>
         <v>-4.7337315749631376E-2</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="28">
         <v>0.37639751552794998</v>
       </c>
       <c r="H8" s="19">
@@ -1005,7 +2017,7 @@
         <f>(I8-Q8)/Q8</f>
         <v>9.4210228320958059E-2</v>
       </c>
-      <c r="K8" s="39">
+      <c r="K8" s="28">
         <v>0.436645962732919</v>
       </c>
       <c r="L8" s="19">
@@ -1035,7 +2047,7 @@
         <f>+(E9-Q9)/Q9</f>
         <v>3.5731885498886853E-2</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="29">
         <v>0.119562000591891</v>
       </c>
       <c r="H9" s="22">
@@ -1049,7 +2061,7 @@
         <f>(I9-Q9)/Q9</f>
         <v>-2.0609201006443551E-2</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K9" s="29">
         <v>0.113873815501741</v>
       </c>
       <c r="L9" s="22">
@@ -1077,23 +2089,23 @@
     </row>
     <row r="12" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27" t="s">
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="O13" s="24" t="s">
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="O13" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="26"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="49"/>
     </row>
     <row r="14" spans="4:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
@@ -1102,19 +2114,19 @@
       <c r="E14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="27" t="s">
         <v>14</v>
       </c>
       <c r="H14" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="J14" s="27" t="s">
         <v>14</v>
       </c>
       <c r="O14" s="9"/>
@@ -1131,23 +2143,23 @@
       <c r="D15" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="25">
         <v>5.9884083325106897E-2</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="24">
         <v>-1.8293715981854121E-2</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="24">
         <f>(E15-Q15)/Q15</f>
         <v>1.4984463137405094E-2</v>
       </c>
-      <c r="H15" s="29">
+      <c r="H15" s="25">
         <v>6.0328851160942401E-2</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I15" s="24">
         <v>-1.100243998455078E-2</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="24">
         <f>(H15-Q15)/Q15</f>
         <v>2.2522901032922107E-2</v>
       </c>
@@ -1167,23 +2179,23 @@
       <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="25">
         <v>0.78537632673401603</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="24">
         <v>1.7555187933877524E-3</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="24">
         <f t="shared" ref="G16:G19" si="0">(E16-Q16)/Q16</f>
         <v>1.6010771971560166E-2</v>
       </c>
-      <c r="H16" s="29">
+      <c r="H16" s="25">
         <v>0.78390557916572101</v>
       </c>
-      <c r="I16" s="28">
+      <c r="I16" s="24">
         <v>-1.2043473760078916E-4</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="24">
         <f t="shared" ref="J16:J19" si="1">(H16-Q16)/Q16</f>
         <v>1.4108123112187568E-2</v>
       </c>
@@ -1203,23 +2215,23 @@
       <c r="D17" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="25">
         <v>6.9088811995386301E-2</v>
       </c>
-      <c r="F17" s="28">
+      <c r="F17" s="24">
         <v>4.6800181748277242E-2</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="24">
         <f t="shared" si="0"/>
         <v>-5.3577917871420473E-2</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="25">
         <v>6.3533105549912205E-2</v>
       </c>
-      <c r="I17" s="28">
+      <c r="I17" s="24">
         <v>-3.7377188637693903E-2</v>
       </c>
-      <c r="J17" s="28">
+      <c r="J17" s="24">
         <f t="shared" si="1"/>
         <v>-0.12968348561764095</v>
       </c>
@@ -1239,23 +2251,23 @@
       <c r="D18" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="25">
         <v>0.431556195965417</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="24">
         <v>-4.7337315749631376E-2</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="24">
         <f t="shared" si="0"/>
         <v>0.26556069198069493</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" s="25">
         <v>0.49567723342939402</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="24">
         <v>9.4210228320958059E-2</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="24">
         <f t="shared" si="1"/>
         <v>0.45359892501288557</v>
       </c>
@@ -1275,23 +2287,23 @@
       <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="25">
         <v>0.11910916683237199</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="24">
         <v>3.5731885498886853E-2</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G19" s="24">
         <f t="shared" si="0"/>
         <v>-7.4236097302333532E-3</v>
       </c>
-      <c r="H19" s="29">
+      <c r="H19" s="25">
         <v>0.112629941884259</v>
       </c>
-      <c r="I19" s="28">
+      <c r="I19" s="24">
         <v>-2.0609201006443551E-2</v>
       </c>
-      <c r="J19" s="28">
+      <c r="J19" s="24">
         <f t="shared" si="1"/>
         <v>-6.1417150964508324E-2</v>
       </c>
@@ -1327,356 +2339,907 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="4:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="33"/>
     </row>
     <row r="25" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="38"/>
     </row>
     <row r="26" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" s="38"/>
     </row>
     <row r="27" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="35">
+        <v>6.0516504052883703E-2</v>
+      </c>
+      <c r="H27" s="35">
+        <v>6.0260712902221701E-2</v>
+      </c>
+      <c r="I27" s="35">
+        <v>5.9405203335232797E-2</v>
+      </c>
+      <c r="J27" s="35">
+        <v>5.9642099860233798E-2</v>
+      </c>
+      <c r="K27" s="35">
+        <v>5.9884083325106897E-2</v>
+      </c>
+      <c r="L27" s="38"/>
     </row>
     <row r="28" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="35">
+        <v>0.78256298069020902</v>
+      </c>
+      <c r="H28" s="35">
+        <v>0.78181338376499498</v>
+      </c>
+      <c r="I28" s="35">
+        <v>0.78364794073197197</v>
+      </c>
+      <c r="J28" s="35">
+        <v>0.78290220916021902</v>
+      </c>
+      <c r="K28" s="35">
+        <v>0.78537632673401603</v>
+      </c>
+      <c r="L28" s="38"/>
     </row>
     <row r="29" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="35">
+        <v>6.4779019956117401E-2</v>
+      </c>
+      <c r="H29" s="35">
+        <v>5.8687872763419399E-2</v>
+      </c>
+      <c r="I29" s="35">
+        <v>6.3850981173423596E-2</v>
+      </c>
+      <c r="J29" s="35">
+        <v>7.1768815496983093E-2</v>
+      </c>
+      <c r="K29" s="35">
+        <v>6.9088811995386301E-2</v>
+      </c>
+      <c r="L29" s="38"/>
     </row>
     <row r="30" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="35">
+        <v>0.44668587896253598</v>
+      </c>
+      <c r="H30" s="35">
+        <v>0.53170028818443804</v>
+      </c>
+      <c r="I30" s="35">
+        <v>0.46181556195965401</v>
+      </c>
+      <c r="J30" s="35">
+        <v>0.32564841498559</v>
+      </c>
+      <c r="K30" s="35">
+        <v>0.431556195965417</v>
+      </c>
+      <c r="L30" s="38"/>
+      <c r="O30" t="s">
+        <v>33</v>
+      </c>
+      <c r="P30" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="31" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="35">
+        <v>0.113149009946162</v>
+      </c>
+      <c r="H31" s="35">
+        <v>0.10570794241925</v>
+      </c>
+      <c r="I31" s="35">
+        <v>0.11219042618360001</v>
+      </c>
+      <c r="J31" s="35">
+        <v>0.117616445485297</v>
+      </c>
+      <c r="K31" s="35">
+        <v>0.11910916683237199</v>
+      </c>
+      <c r="L31" s="38"/>
+      <c r="O31" t="s">
+        <v>35</v>
+      </c>
+      <c r="P31" s="60">
+        <v>0.88500000000000001</v>
+      </c>
     </row>
     <row r="32" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E32" s="34"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="38"/>
+      <c r="O32" t="s">
+        <v>37</v>
+      </c>
+      <c r="P32" s="60">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E33" s="34"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="38"/>
+      <c r="O33" t="s">
+        <v>38</v>
+      </c>
+      <c r="P33" s="60">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="34" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E34" s="34"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="38"/>
+      <c r="O34" t="s">
+        <v>36</v>
+      </c>
+      <c r="P34" s="60">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E35" s="34"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="J35" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="K35" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="L35" s="38"/>
+    </row>
+    <row r="36" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E36" s="34"/>
+      <c r="F36" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="39">
+        <f>+(G27-$Q5)/$Q5</f>
+        <v>-7.9261630674802557E-3</v>
+      </c>
+      <c r="H36" s="39">
+        <f t="shared" ref="H36:K36" si="2">+(H27-$Q5)/$Q5</f>
+        <v>-1.2119460619316354E-2</v>
+      </c>
+      <c r="I36" s="39">
+        <f t="shared" si="2"/>
+        <v>-2.6144207619134462E-2</v>
+      </c>
+      <c r="J36" s="39">
+        <f t="shared" si="2"/>
+        <v>-2.2260658028954113E-2</v>
+      </c>
+      <c r="K36" s="39">
+        <f t="shared" si="2"/>
+        <v>-1.8293715981854121E-2</v>
+      </c>
+      <c r="L36" s="38"/>
+    </row>
+    <row r="37" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E37" s="34"/>
+      <c r="F37" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="39">
+        <f t="shared" ref="G37:K37" si="3">+(G28-$Q6)/$Q6</f>
+        <v>-1.832932793100778E-3</v>
+      </c>
+      <c r="H37" s="39">
+        <f t="shared" si="3"/>
+        <v>-2.7890513201594969E-3</v>
+      </c>
+      <c r="I37" s="39">
+        <f t="shared" si="3"/>
+        <v>-4.4905518881130081E-4</v>
+      </c>
+      <c r="J37" s="39">
+        <f t="shared" si="3"/>
+        <v>-1.4002434180880228E-3</v>
+      </c>
+      <c r="K37" s="39">
+        <f t="shared" si="3"/>
+        <v>1.7555187933877524E-3</v>
+      </c>
+      <c r="L37" s="38"/>
+    </row>
+    <row r="38" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E38" s="34"/>
+      <c r="F38" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="39">
+        <f t="shared" ref="G38:K38" si="4">+(G29-$Q7)/$Q7</f>
+        <v>-1.8499697634584884E-2</v>
+      </c>
+      <c r="H38" s="39">
+        <f t="shared" si="4"/>
+        <v>-0.11078980661485763</v>
+      </c>
+      <c r="I38" s="39">
+        <f t="shared" si="4"/>
+        <v>-3.2560891311763741E-2</v>
+      </c>
+      <c r="J38" s="39">
+        <f t="shared" si="4"/>
+        <v>8.7406295408834697E-2</v>
+      </c>
+      <c r="K38" s="39">
+        <f t="shared" si="4"/>
+        <v>4.6800181748277242E-2</v>
+      </c>
+      <c r="L38" s="38"/>
+    </row>
+    <row r="39" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E39" s="34"/>
+      <c r="F39" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="39">
+        <f t="shared" ref="G39:K39" si="5">+(G30-$Q8)/$Q8</f>
+        <v>-1.3938457036344453E-2</v>
+      </c>
+      <c r="H39" s="39">
+        <f t="shared" si="5"/>
+        <v>0.17373132049544818</v>
+      </c>
+      <c r="I39" s="39">
+        <f t="shared" si="5"/>
+        <v>1.9460401676940384E-2</v>
+      </c>
+      <c r="J39" s="39">
+        <f t="shared" si="5"/>
+        <v>-0.28112932674262697</v>
+      </c>
+      <c r="K39" s="39">
+        <f t="shared" si="5"/>
+        <v>-4.7337315749631376E-2</v>
+      </c>
+      <c r="L39" s="38"/>
+    </row>
+    <row r="40" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-    </row>
-    <row r="41" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E40" s="34"/>
+      <c r="F40" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="G40" s="39">
+        <f t="shared" ref="G40:K40" si="6">+(G31-$Q9)/$Q9</f>
+        <v>-1.6095565685547829E-2</v>
+      </c>
+      <c r="H40" s="39">
+        <f t="shared" si="6"/>
+        <v>-8.0800500702173997E-2</v>
+      </c>
+      <c r="I40" s="39">
+        <f t="shared" si="6"/>
+        <v>-2.4431076664347816E-2</v>
+      </c>
+      <c r="J40" s="39">
+        <f t="shared" si="6"/>
+        <v>2.2751699872147757E-2</v>
+      </c>
+      <c r="K40" s="39">
+        <f t="shared" si="6"/>
+        <v>3.5731885498886853E-2</v>
+      </c>
+      <c r="L40" s="38"/>
+    </row>
+    <row r="41" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E41" s="34"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="38"/>
+    </row>
+    <row r="42" spans="4:16" x14ac:dyDescent="0.3">
       <c r="D42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="4:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="35"/>
-      <c r="E43" s="36" t="s">
+      <c r="E42" s="34"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="38"/>
+    </row>
+    <row r="43" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="51"/>
+      <c r="E43" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="36" t="s">
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
+      <c r="J43" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="36"/>
-    </row>
-    <row r="44" spans="4:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="35"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="35"/>
-      <c r="N44" s="36"/>
-    </row>
-    <row r="45" spans="4:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="36" t="s">
+      <c r="K43" s="54"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="52"/>
+    </row>
+    <row r="44" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="51"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="54"/>
+      <c r="K44" s="54"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="52"/>
+    </row>
+    <row r="45" spans="4:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="36" t="s">
+      <c r="E45" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="F45" s="34" t="s">
+      <c r="F45" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="34" t="s">
+      <c r="G45" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="I45" s="34" t="s">
+      <c r="I45" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="J45" s="34" t="s">
+      <c r="J45" s="40" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="4:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="33"/>
-      <c r="J46" s="33"/>
-    </row>
-    <row r="47" spans="4:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="34" t="s">
+      <c r="K45" s="35"/>
+      <c r="L45" s="38"/>
+    </row>
+    <row r="46" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="52"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="41"/>
+      <c r="H46" s="54"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="38"/>
+    </row>
+    <row r="47" spans="4:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="52"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="G47" s="34" t="s">
+      <c r="G47" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="H47" s="36"/>
-      <c r="I47" s="34" t="s">
+      <c r="H47" s="54"/>
+      <c r="I47" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="J47" s="34" t="s">
+      <c r="J47" s="40" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="4:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-    </row>
-    <row r="49" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="36" t="s">
+      <c r="K47" s="35"/>
+      <c r="L47" s="38"/>
+    </row>
+    <row r="48" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="52"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="38"/>
+    </row>
+    <row r="49" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="E49" s="37">
+      <c r="E49" s="58">
         <v>0.06</v>
       </c>
-      <c r="F49" s="38">
+      <c r="F49" s="57">
         <v>-1.83E-2</v>
       </c>
-      <c r="G49" s="38">
+      <c r="G49" s="57">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="H49" s="37">
+      <c r="H49" s="59">
         <v>0.06</v>
       </c>
-      <c r="I49" s="38">
+      <c r="I49" s="57">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="J49" s="38">
+      <c r="J49" s="57">
         <v>2.2499999999999999E-2</v>
       </c>
-    </row>
-    <row r="50" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="36"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="38"/>
-      <c r="J50" s="38"/>
-    </row>
-    <row r="51" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="36" t="s">
+      <c r="K49" s="35"/>
+      <c r="L49" s="38"/>
+    </row>
+    <row r="50" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="52"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="57"/>
+      <c r="J50" s="57"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="38"/>
+    </row>
+    <row r="51" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D51" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="E51" s="37">
+      <c r="E51" s="58">
         <v>0.78500000000000003</v>
       </c>
-      <c r="F51" s="38">
+      <c r="F51" s="57">
         <v>1.8E-3</v>
       </c>
-      <c r="G51" s="38">
+      <c r="G51" s="57">
         <v>1.6E-2</v>
       </c>
-      <c r="H51" s="37">
+      <c r="H51" s="59">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I51" s="38">
+      <c r="I51" s="57">
         <v>-1E-4</v>
       </c>
-      <c r="J51" s="38">
+      <c r="J51" s="57">
         <v>1.41E-2</v>
       </c>
-    </row>
-    <row r="52" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="36"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="38"/>
-    </row>
-    <row r="53" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="36" t="s">
+      <c r="K51" s="35"/>
+      <c r="L51" s="38"/>
+    </row>
+    <row r="52" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="52"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="38"/>
+    </row>
+    <row r="53" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E53" s="37">
+      <c r="E53" s="58">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="F53" s="38">
+      <c r="F53" s="57">
         <v>4.6800000000000001E-2</v>
       </c>
-      <c r="G53" s="38">
+      <c r="G53" s="57">
         <v>-5.3600000000000002E-2</v>
       </c>
-      <c r="H53" s="37">
+      <c r="H53" s="59">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="I53" s="38">
+      <c r="I53" s="57">
         <v>-3.7400000000000003E-2</v>
       </c>
-      <c r="J53" s="38">
+      <c r="J53" s="57">
         <v>-0.12970000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="36"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="38"/>
-    </row>
-    <row r="55" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="36" t="s">
+      <c r="K53" s="35"/>
+      <c r="L53" s="38"/>
+    </row>
+    <row r="54" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="52"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="57"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="57"/>
+      <c r="J54" s="57"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="38"/>
+    </row>
+    <row r="55" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="37">
+      <c r="E55" s="58">
         <v>0.432</v>
       </c>
-      <c r="F55" s="38">
+      <c r="F55" s="57">
         <v>-4.7300000000000002E-2</v>
       </c>
-      <c r="G55" s="38">
+      <c r="G55" s="57">
         <v>0.2656</v>
       </c>
-      <c r="H55" s="37">
+      <c r="H55" s="59">
         <v>0.496</v>
       </c>
-      <c r="I55" s="38">
+      <c r="I55" s="57">
         <v>9.4200000000000006E-2</v>
       </c>
-      <c r="J55" s="38">
+      <c r="J55" s="57">
         <v>0.4536</v>
       </c>
-    </row>
-    <row r="56" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="36"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="38"/>
-      <c r="J56" s="38"/>
-    </row>
-    <row r="57" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="36" t="s">
+      <c r="K55" s="35"/>
+      <c r="L55" s="38"/>
+    </row>
+    <row r="56" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="52"/>
+      <c r="E56" s="58"/>
+      <c r="F56" s="57"/>
+      <c r="G56" s="57"/>
+      <c r="H56" s="59"/>
+      <c r="I56" s="57"/>
+      <c r="J56" s="57"/>
+      <c r="K56" s="35"/>
+      <c r="L56" s="38"/>
+    </row>
+    <row r="57" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="E57" s="37">
+      <c r="E57" s="58">
         <v>0.11899999999999999</v>
       </c>
-      <c r="F57" s="38">
+      <c r="F57" s="57">
         <v>3.5700000000000003E-2</v>
       </c>
-      <c r="G57" s="38">
+      <c r="G57" s="57">
         <v>-7.4000000000000003E-3</v>
       </c>
-      <c r="H57" s="37">
+      <c r="H57" s="59">
         <v>0.113</v>
       </c>
-      <c r="I57" s="38">
+      <c r="I57" s="57">
         <v>-2.06E-2</v>
       </c>
-      <c r="J57" s="38">
+      <c r="J57" s="57">
         <v>-6.1400000000000003E-2</v>
       </c>
-    </row>
-    <row r="58" spans="4:10" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="36"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="38"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="38"/>
+      <c r="K57" s="35"/>
+      <c r="L57" s="38"/>
+    </row>
+    <row r="58" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D58" s="52"/>
+      <c r="E58" s="58"/>
+      <c r="F58" s="57"/>
+      <c r="G58" s="57"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="57"/>
+      <c r="J58" s="57"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="38"/>
+    </row>
+    <row r="59" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="E59" s="34"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="46"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="38"/>
+    </row>
+    <row r="60" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="E60" s="34"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H60" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I60" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="J60" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="K60" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="L60" s="38"/>
+    </row>
+    <row r="61" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="E61" s="34"/>
+      <c r="F61" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G61" s="39">
+        <f>+(G27-$Q15)/$Q15</f>
+        <v>2.5703458523452648E-2</v>
+      </c>
+      <c r="H61" s="39">
+        <f t="shared" ref="H61:K61" si="7">+(H27-$Q15)/$Q15</f>
+        <v>2.1368015291893295E-2</v>
+      </c>
+      <c r="I61" s="39">
+        <f t="shared" si="7"/>
+        <v>6.8678531395389777E-3</v>
+      </c>
+      <c r="J61" s="39">
+        <f t="shared" si="7"/>
+        <v>1.0883048478539001E-2</v>
+      </c>
+      <c r="K61" s="39">
+        <f t="shared" si="7"/>
+        <v>1.4984463137405094E-2</v>
+      </c>
+      <c r="L61" s="38"/>
+    </row>
+    <row r="62" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="E62" s="34"/>
+      <c r="F62" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G62" s="39">
+        <f t="shared" ref="G62:K62" si="8">+(G28-$Q16)/$Q16</f>
+        <v>1.2371255744125485E-2</v>
+      </c>
+      <c r="H62" s="39">
+        <f t="shared" si="8"/>
+        <v>1.1401531390679126E-2</v>
+      </c>
+      <c r="I62" s="39">
+        <f t="shared" si="8"/>
+        <v>1.37748263026804E-2</v>
+      </c>
+      <c r="J62" s="39">
+        <f t="shared" si="8"/>
+        <v>1.2810102406492885E-2</v>
+      </c>
+      <c r="K62" s="39">
+        <f t="shared" si="8"/>
+        <v>1.6010771971560166E-2</v>
+      </c>
+      <c r="L62" s="38"/>
+    </row>
+    <row r="63" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="E63" s="34"/>
+      <c r="F63" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="G63" s="39">
+        <f t="shared" ref="G63:K63" si="9">+(G29-$Q17)/$Q17</f>
+        <v>-0.11261616498469308</v>
+      </c>
+      <c r="H63" s="39">
+        <f t="shared" si="9"/>
+        <v>-0.19605653748740545</v>
+      </c>
+      <c r="I63" s="39">
+        <f t="shared" si="9"/>
+        <v>-0.12532902502159451</v>
+      </c>
+      <c r="J63" s="39">
+        <f t="shared" si="9"/>
+        <v>-1.6865541137217839E-2</v>
+      </c>
+      <c r="K63" s="39">
+        <f t="shared" si="9"/>
+        <v>-5.3577917871420473E-2</v>
+      </c>
+      <c r="L63" s="38"/>
+    </row>
+    <row r="64" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="E64" s="34"/>
+      <c r="F64" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G64" s="39">
+        <f t="shared" ref="G64:K64" si="10">+(G30-$Q18)/$Q18</f>
+        <v>0.3099292638197535</v>
+      </c>
+      <c r="H64" s="39">
+        <f t="shared" si="10"/>
+        <v>0.55923838177254548</v>
+      </c>
+      <c r="I64" s="39">
+        <f t="shared" si="10"/>
+        <v>0.35429783565880929</v>
+      </c>
+      <c r="J64" s="39">
+        <f t="shared" si="10"/>
+        <v>-4.5019310892698033E-2</v>
+      </c>
+      <c r="K64" s="39">
+        <f t="shared" si="10"/>
+        <v>0.26556069198069493</v>
+      </c>
+      <c r="L64" s="38"/>
+    </row>
+    <row r="65" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E65" s="34"/>
+      <c r="F65" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" s="39">
+        <f t="shared" ref="G65:K65" si="11">+(G31-$Q19)/$Q19</f>
+        <v>-5.7091583781983257E-2</v>
+      </c>
+      <c r="H65" s="39">
+        <f t="shared" si="11"/>
+        <v>-0.11910047983958334</v>
+      </c>
+      <c r="I65" s="39">
+        <f t="shared" si="11"/>
+        <v>-6.507978180333325E-2</v>
+      </c>
+      <c r="J65" s="39">
+        <f t="shared" si="11"/>
+        <v>-1.9862954289191655E-2</v>
+      </c>
+      <c r="K65" s="39">
+        <f t="shared" si="11"/>
+        <v>-7.4236097302333532E-3</v>
+      </c>
+      <c r="L65" s="38"/>
+    </row>
+    <row r="66" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E66" s="34"/>
+      <c r="F66" s="35"/>
+      <c r="G66" s="35"/>
+      <c r="H66" s="35"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="35"/>
+      <c r="K66" s="35"/>
+      <c r="L66" s="38"/>
+    </row>
+    <row r="67" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E67" s="34"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="35"/>
+      <c r="K67" s="35"/>
+      <c r="L67" s="38"/>
+    </row>
+    <row r="68" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E68" s="34"/>
+      <c r="F68" s="35"/>
+      <c r="G68" s="35"/>
+      <c r="H68" s="35"/>
+      <c r="I68" s="35"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="35"/>
+      <c r="L68" s="38"/>
+    </row>
+    <row r="69" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E69" s="43"/>
+      <c r="F69" s="44"/>
+      <c r="G69" s="44"/>
+      <c r="H69" s="44"/>
+      <c r="I69" s="44"/>
+      <c r="J69" s="44"/>
+      <c r="K69" s="44"/>
+      <c r="L69" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O31:P34">
+    <sortCondition descending="1" ref="P31:P34"/>
+  </sortState>
+  <mergeCells count="53">
     <mergeCell ref="I57:I58"/>
     <mergeCell ref="J57:J58"/>
     <mergeCell ref="D57:D58"/>
@@ -1698,38 +3261,41 @@
     <mergeCell ref="F53:F54"/>
     <mergeCell ref="G53:G54"/>
     <mergeCell ref="H53:H54"/>
-    <mergeCell ref="I49:I50"/>
-    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="E51:E52"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="G51:G52"/>
     <mergeCell ref="H51:H52"/>
-    <mergeCell ref="I51:I52"/>
-    <mergeCell ref="J51:J52"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="N43:N44"/>
     <mergeCell ref="D45:D48"/>
     <mergeCell ref="E45:E48"/>
     <mergeCell ref="H45:H48"/>
     <mergeCell ref="D43:D44"/>
     <mergeCell ref="E43:G44"/>
     <mergeCell ref="H43:H44"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="J43:L44"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="G59:K59"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="O3:S3"/>
     <mergeCell ref="O13:S13"/>
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="H13:J13"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="N43:N44"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="J43:L44"/>
+    <mergeCell ref="I49:I50"/>
+    <mergeCell ref="J49:J50"/>
+    <mergeCell ref="I51:I52"/>
+    <mergeCell ref="J51:J52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualiza repositorio con los codigos y salidas correspondientes al tercer trabajo
</commit_message>
<xml_diff>
--- a/data/Resultados_AG.xlsx
+++ b/data/Resultados_AG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasal\Google Drive\EAFIT\Ciencia de Datos y Analitica\03 Tercer Semestre\Metodos Heuristicos para Optimizacion\metodos-heuristicos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7860BD67-FAC4-4E54-BEC1-09B8F2DEC368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD21EC6B-A900-4A58-A179-7D60A6733380}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B1250CC-1120-467C-8907-0AF514310821}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B1250CC-1120-467C-8907-0AF514310821}"/>
   </bookViews>
   <sheets>
     <sheet name="AG" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
   <si>
     <t>Precision</t>
   </si>
@@ -150,15 +150,32 @@
   </si>
   <si>
     <t>Tanh</t>
+  </si>
+  <si>
+    <t>Tiempo cómputo</t>
+  </si>
+  <si>
+    <t>Fitness</t>
+  </si>
+  <si>
+    <t>Tiempo cómputo (mins)</t>
+  </si>
+  <si>
+    <t>DF peor solución</t>
+  </si>
+  <si>
+    <t>DP mejor solución</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="173" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -407,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -498,6 +515,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -513,34 +555,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1781,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0DA66-6DF4-4FA4-8913-44EB5171D2D4}">
-  <dimension ref="D2:S69"/>
+  <dimension ref="D2:S77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G28" workbookViewId="0">
-      <selection activeCell="T42" sqref="T42"/>
+    <sheetView tabSelected="1" topLeftCell="D39" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1802,25 +1823,25 @@
   <sheetData>
     <row r="2" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="47" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="49"/>
-      <c r="O3" s="47" t="s">
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="58"/>
+      <c r="O3" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="49"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
+      <c r="R3" s="57"/>
+      <c r="S3" s="58"/>
     </row>
     <row r="4" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
@@ -2089,23 +2110,23 @@
     </row>
     <row r="12" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50" t="s">
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="O13" s="47" t="s">
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="O13" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="49"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="58"/>
     </row>
     <row r="14" spans="4:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
@@ -2395,20 +2416,20 @@
       <c r="F27" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="35">
-        <v>6.0516504052883703E-2</v>
-      </c>
-      <c r="H27" s="35">
-        <v>6.0260712902221701E-2</v>
-      </c>
-      <c r="I27" s="35">
-        <v>5.9405203335232797E-2</v>
-      </c>
-      <c r="J27" s="35">
-        <v>5.9642099860233798E-2</v>
-      </c>
-      <c r="K27" s="35">
-        <v>5.9884083325106897E-2</v>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
       </c>
       <c r="L27" s="38"/>
     </row>
@@ -2418,19 +2439,19 @@
       <c r="F28" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="35">
-        <v>0.78256298069020902</v>
-      </c>
-      <c r="H28" s="35">
-        <v>0.78181338376499498</v>
-      </c>
-      <c r="I28" s="35">
-        <v>0.78364794073197197</v>
-      </c>
-      <c r="J28" s="35">
-        <v>0.78290220916021902</v>
-      </c>
-      <c r="K28" s="35">
+      <c r="G28">
+        <v>0.78402478355865801</v>
+      </c>
+      <c r="H28">
+        <v>0.78320749438814696</v>
+      </c>
+      <c r="I28">
+        <v>0.78275763717119595</v>
+      </c>
+      <c r="J28">
+        <v>0.78348144888675997</v>
+      </c>
+      <c r="K28">
         <v>0.78537632673401603</v>
       </c>
       <c r="L28" s="38"/>
@@ -2441,20 +2462,20 @@
       <c r="F29" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="G29" s="35">
-        <v>6.4779019956117401E-2</v>
-      </c>
-      <c r="H29" s="35">
-        <v>5.8687872763419399E-2</v>
-      </c>
-      <c r="I29" s="35">
-        <v>6.3850981173423596E-2</v>
-      </c>
-      <c r="J29" s="35">
-        <v>7.1768815496983093E-2</v>
-      </c>
-      <c r="K29" s="35">
-        <v>6.9088811995386301E-2</v>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
       </c>
       <c r="L29" s="38"/>
     </row>
@@ -2464,20 +2485,20 @@
       <c r="F30" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="35">
-        <v>0.44668587896253598</v>
-      </c>
-      <c r="H30" s="35">
-        <v>0.53170028818443804</v>
-      </c>
-      <c r="I30" s="35">
-        <v>0.46181556195965401</v>
-      </c>
-      <c r="J30" s="35">
-        <v>0.32564841498559</v>
-      </c>
-      <c r="K30" s="35">
-        <v>0.431556195965417</v>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
       </c>
       <c r="L30" s="38"/>
       <c r="O30" t="s">
@@ -2493,43 +2514,56 @@
       <c r="F31" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="35">
-        <v>0.113149009946162</v>
-      </c>
-      <c r="H31" s="35">
-        <v>0.10570794241925</v>
-      </c>
-      <c r="I31" s="35">
-        <v>0.11219042618360001</v>
-      </c>
-      <c r="J31" s="35">
-        <v>0.117616445485297</v>
-      </c>
-      <c r="K31" s="35">
-        <v>0.11910916683237199</v>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
       </c>
       <c r="L31" s="38"/>
       <c r="O31" t="s">
         <v>35</v>
       </c>
-      <c r="P31" s="60">
+      <c r="P31" s="46">
         <v>0.88500000000000001</v>
       </c>
     </row>
     <row r="32" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D32" s="1"/>
       <c r="E32" s="34"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="35"/>
+      <c r="F32" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="63">
+        <v>382.23689426581001</v>
+      </c>
+      <c r="H32" s="64">
+        <v>409.63159538507398</v>
+      </c>
+      <c r="I32" s="64">
+        <v>389.84634193181898</v>
+      </c>
+      <c r="J32" s="64">
+        <v>419.084818784395</v>
+      </c>
+      <c r="K32" s="64">
+        <f>370.970108131567</f>
+        <v>370.97010813156697</v>
+      </c>
       <c r="L32" s="38"/>
       <c r="O32" t="s">
         <v>37</v>
       </c>
-      <c r="P32" s="60">
+      <c r="P32" s="46">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -2546,7 +2580,7 @@
       <c r="O33" t="s">
         <v>38</v>
       </c>
-      <c r="P33" s="60">
+      <c r="P33" s="46">
         <v>0.03</v>
       </c>
     </row>
@@ -2554,18 +2588,18 @@
       <c r="D34" s="1"/>
       <c r="E34" s="34"/>
       <c r="F34" s="35"/>
-      <c r="G34" s="46" t="s">
+      <c r="G34" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
       <c r="L34" s="38"/>
       <c r="O34" t="s">
         <v>36</v>
       </c>
-      <c r="P34" s="60">
+      <c r="P34" s="46">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -2598,23 +2632,23 @@
       </c>
       <c r="G36" s="39">
         <f>+(G27-$Q5)/$Q5</f>
-        <v>-7.9261630674802557E-3</v>
+        <v>-1</v>
       </c>
       <c r="H36" s="39">
         <f t="shared" ref="H36:K36" si="2">+(H27-$Q5)/$Q5</f>
-        <v>-1.2119460619316354E-2</v>
+        <v>-1</v>
       </c>
       <c r="I36" s="39">
         <f t="shared" si="2"/>
-        <v>-2.6144207619134462E-2</v>
+        <v>-1</v>
       </c>
       <c r="J36" s="39">
         <f t="shared" si="2"/>
-        <v>-2.2260658028954113E-2</v>
+        <v>-1</v>
       </c>
       <c r="K36" s="39">
         <f t="shared" si="2"/>
-        <v>-1.8293715981854121E-2</v>
+        <v>-1</v>
       </c>
       <c r="L36" s="38"/>
     </row>
@@ -2625,20 +2659,20 @@
         <v>2</v>
       </c>
       <c r="G37" s="39">
-        <f t="shared" ref="G37:K37" si="3">+(G28-$Q6)/$Q6</f>
-        <v>-1.832932793100778E-3</v>
+        <f>+(G28-$Q6)/$Q6</f>
+        <v>3.1611681961711006E-5</v>
       </c>
       <c r="H37" s="39">
-        <f t="shared" si="3"/>
-        <v>-2.7890513201594969E-3</v>
+        <f t="shared" ref="H37:K37" si="3">+(H28-$Q6)/$Q6</f>
+        <v>-1.0108489947105448E-3</v>
       </c>
       <c r="I37" s="39">
         <f t="shared" si="3"/>
-        <v>-4.4905518881130081E-4</v>
+        <v>-1.5846464653113236E-3</v>
       </c>
       <c r="J37" s="39">
         <f t="shared" si="3"/>
-        <v>-1.4002434180880228E-3</v>
+        <v>-6.6141723627558956E-4</v>
       </c>
       <c r="K37" s="39">
         <f t="shared" si="3"/>
@@ -2653,24 +2687,24 @@
         <v>0</v>
       </c>
       <c r="G38" s="39">
-        <f t="shared" ref="G38:K38" si="4">+(G29-$Q7)/$Q7</f>
-        <v>-1.8499697634584884E-2</v>
+        <f>+(G29-$Q7)/$Q7</f>
+        <v>-1</v>
       </c>
       <c r="H38" s="39">
-        <f t="shared" si="4"/>
-        <v>-0.11078980661485763</v>
+        <f t="shared" ref="H38:K38" si="4">+(H29-$Q7)/$Q7</f>
+        <v>-1</v>
       </c>
       <c r="I38" s="39">
         <f t="shared" si="4"/>
-        <v>-3.2560891311763741E-2</v>
+        <v>-1</v>
       </c>
       <c r="J38" s="39">
         <f t="shared" si="4"/>
-        <v>8.7406295408834697E-2</v>
+        <v>-1</v>
       </c>
       <c r="K38" s="39">
         <f t="shared" si="4"/>
-        <v>4.6800181748277242E-2</v>
+        <v>-1</v>
       </c>
       <c r="L38" s="38"/>
     </row>
@@ -2681,24 +2715,24 @@
         <v>3</v>
       </c>
       <c r="G39" s="39">
-        <f t="shared" ref="G39:K39" si="5">+(G30-$Q8)/$Q8</f>
-        <v>-1.3938457036344453E-2</v>
+        <f>+(G30-$Q8)/$Q8</f>
+        <v>-1</v>
       </c>
       <c r="H39" s="39">
-        <f t="shared" si="5"/>
-        <v>0.17373132049544818</v>
+        <f t="shared" ref="H39:K39" si="5">+(H30-$Q8)/$Q8</f>
+        <v>-1</v>
       </c>
       <c r="I39" s="39">
         <f t="shared" si="5"/>
-        <v>1.9460401676940384E-2</v>
+        <v>-1</v>
       </c>
       <c r="J39" s="39">
         <f t="shared" si="5"/>
-        <v>-0.28112932674262697</v>
+        <v>-1</v>
       </c>
       <c r="K39" s="39">
         <f t="shared" si="5"/>
-        <v>-4.7337315749631376E-2</v>
+        <v>-1</v>
       </c>
       <c r="L39" s="38"/>
     </row>
@@ -2709,24 +2743,24 @@
         <v>32</v>
       </c>
       <c r="G40" s="39">
-        <f t="shared" ref="G40:K40" si="6">+(G31-$Q9)/$Q9</f>
-        <v>-1.6095565685547829E-2</v>
+        <f>+(G31-$Q9)/$Q9</f>
+        <v>-1</v>
       </c>
       <c r="H40" s="39">
-        <f t="shared" si="6"/>
-        <v>-8.0800500702173997E-2</v>
+        <f t="shared" ref="H40:K40" si="6">+(H31-$Q9)/$Q9</f>
+        <v>-1</v>
       </c>
       <c r="I40" s="39">
         <f t="shared" si="6"/>
-        <v>-2.4431076664347816E-2</v>
+        <v>-1</v>
       </c>
       <c r="J40" s="39">
         <f t="shared" si="6"/>
-        <v>2.2751699872147757E-2</v>
+        <v>-1</v>
       </c>
       <c r="K40" s="39">
         <f t="shared" si="6"/>
-        <v>3.5731885498886853E-2</v>
+        <v>-1</v>
       </c>
       <c r="L40" s="38"/>
     </row>
@@ -2753,40 +2787,40 @@
       <c r="L42" s="38"/>
     </row>
     <row r="43" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="51"/>
-      <c r="E43" s="53" t="s">
+      <c r="D43" s="53"/>
+      <c r="E43" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="55"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="54" t="s">
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="K43" s="54"/>
-      <c r="L43" s="56"/>
-      <c r="M43" s="51"/>
-      <c r="N43" s="52"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="60"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="48"/>
     </row>
     <row r="44" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="51"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="54"/>
-      <c r="K44" s="54"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="52"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="60"/>
+      <c r="M44" s="53"/>
+      <c r="N44" s="48"/>
     </row>
     <row r="45" spans="4:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="52" t="s">
+      <c r="D45" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="53" t="s">
+      <c r="E45" s="51" t="s">
         <v>19</v>
       </c>
       <c r="F45" s="40" t="s">
@@ -2795,7 +2829,7 @@
       <c r="G45" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="54" t="s">
+      <c r="H45" s="52" t="s">
         <v>19</v>
       </c>
       <c r="I45" s="40" t="s">
@@ -2808,26 +2842,26 @@
       <c r="L45" s="38"/>
     </row>
     <row r="46" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="52"/>
-      <c r="E46" s="53"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="51"/>
       <c r="F46" s="41"/>
       <c r="G46" s="41"/>
-      <c r="H46" s="54"/>
+      <c r="H46" s="52"/>
       <c r="I46" s="41"/>
       <c r="J46" s="41"/>
       <c r="K46" s="35"/>
       <c r="L46" s="38"/>
     </row>
     <row r="47" spans="4:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="52"/>
-      <c r="E47" s="53"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="51"/>
       <c r="F47" s="40" t="s">
         <v>21</v>
       </c>
       <c r="G47" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="H47" s="54"/>
+      <c r="H47" s="52"/>
       <c r="I47" s="40" t="s">
         <v>21</v>
       </c>
@@ -2838,206 +2872,206 @@
       <c r="L47" s="38"/>
     </row>
     <row r="48" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="52"/>
-      <c r="E48" s="53"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="51"/>
       <c r="F48" s="42"/>
       <c r="G48" s="42"/>
-      <c r="H48" s="54"/>
+      <c r="H48" s="52"/>
       <c r="I48" s="42"/>
       <c r="J48" s="42"/>
       <c r="K48" s="35"/>
       <c r="L48" s="38"/>
     </row>
     <row r="49" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="52" t="s">
+      <c r="D49" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="E49" s="58">
+      <c r="E49" s="49">
         <v>0.06</v>
       </c>
-      <c r="F49" s="57">
+      <c r="F49" s="47">
         <v>-1.83E-2</v>
       </c>
-      <c r="G49" s="57">
+      <c r="G49" s="47">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="H49" s="59">
+      <c r="H49" s="50">
         <v>0.06</v>
       </c>
-      <c r="I49" s="57">
+      <c r="I49" s="47">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="J49" s="57">
+      <c r="J49" s="47">
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="K49" s="35"/>
       <c r="L49" s="38"/>
     </row>
     <row r="50" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="52"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="47"/>
       <c r="K50" s="35"/>
       <c r="L50" s="38"/>
     </row>
     <row r="51" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="52" t="s">
+      <c r="D51" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E51" s="58">
+      <c r="E51" s="49">
         <v>0.78500000000000003</v>
       </c>
-      <c r="F51" s="57">
+      <c r="F51" s="47">
         <v>1.8E-3</v>
       </c>
-      <c r="G51" s="57">
+      <c r="G51" s="47">
         <v>1.6E-2</v>
       </c>
-      <c r="H51" s="59">
+      <c r="H51" s="50">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I51" s="57">
+      <c r="I51" s="47">
         <v>-1E-4</v>
       </c>
-      <c r="J51" s="57">
+      <c r="J51" s="47">
         <v>1.41E-2</v>
       </c>
       <c r="K51" s="35"/>
       <c r="L51" s="38"/>
     </row>
     <row r="52" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="52"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="47"/>
+      <c r="J52" s="47"/>
       <c r="K52" s="35"/>
       <c r="L52" s="38"/>
     </row>
     <row r="53" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="52" t="s">
+      <c r="D53" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="E53" s="58">
+      <c r="E53" s="49">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="F53" s="57">
+      <c r="F53" s="47">
         <v>4.6800000000000001E-2</v>
       </c>
-      <c r="G53" s="57">
+      <c r="G53" s="47">
         <v>-5.3600000000000002E-2</v>
       </c>
-      <c r="H53" s="59">
+      <c r="H53" s="50">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="I53" s="57">
+      <c r="I53" s="47">
         <v>-3.7400000000000003E-2</v>
       </c>
-      <c r="J53" s="57">
+      <c r="J53" s="47">
         <v>-0.12970000000000001</v>
       </c>
       <c r="K53" s="35"/>
       <c r="L53" s="38"/>
     </row>
     <row r="54" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="52"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="57"/>
-      <c r="H54" s="59"/>
-      <c r="I54" s="57"/>
-      <c r="J54" s="57"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="47"/>
+      <c r="H54" s="50"/>
+      <c r="I54" s="47"/>
+      <c r="J54" s="47"/>
       <c r="K54" s="35"/>
       <c r="L54" s="38"/>
     </row>
     <row r="55" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="52" t="s">
+      <c r="D55" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="58">
+      <c r="E55" s="49">
         <v>0.432</v>
       </c>
-      <c r="F55" s="57">
+      <c r="F55" s="47">
         <v>-4.7300000000000002E-2</v>
       </c>
-      <c r="G55" s="57">
+      <c r="G55" s="47">
         <v>0.2656</v>
       </c>
-      <c r="H55" s="59">
+      <c r="H55" s="50">
         <v>0.496</v>
       </c>
-      <c r="I55" s="57">
+      <c r="I55" s="47">
         <v>9.4200000000000006E-2</v>
       </c>
-      <c r="J55" s="57">
+      <c r="J55" s="47">
         <v>0.4536</v>
       </c>
       <c r="K55" s="35"/>
       <c r="L55" s="38"/>
     </row>
     <row r="56" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="52"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="57"/>
-      <c r="H56" s="59"/>
-      <c r="I56" s="57"/>
-      <c r="J56" s="57"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="50"/>
+      <c r="I56" s="47"/>
+      <c r="J56" s="47"/>
       <c r="K56" s="35"/>
       <c r="L56" s="38"/>
     </row>
     <row r="57" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="52" t="s">
+      <c r="D57" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E57" s="58">
+      <c r="E57" s="49">
         <v>0.11899999999999999</v>
       </c>
-      <c r="F57" s="57">
+      <c r="F57" s="47">
         <v>3.5700000000000003E-2</v>
       </c>
-      <c r="G57" s="57">
+      <c r="G57" s="47">
         <v>-7.4000000000000003E-3</v>
       </c>
-      <c r="H57" s="59">
+      <c r="H57" s="50">
         <v>0.113</v>
       </c>
-      <c r="I57" s="57">
+      <c r="I57" s="47">
         <v>-2.06E-2</v>
       </c>
-      <c r="J57" s="57">
+      <c r="J57" s="47">
         <v>-6.1400000000000003E-2</v>
       </c>
       <c r="K57" s="35"/>
       <c r="L57" s="38"/>
     </row>
     <row r="58" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="52"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="57"/>
-      <c r="G58" s="57"/>
-      <c r="H58" s="59"/>
-      <c r="I58" s="57"/>
-      <c r="J58" s="57"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="50"/>
+      <c r="I58" s="47"/>
+      <c r="J58" s="47"/>
       <c r="K58" s="35"/>
       <c r="L58" s="38"/>
     </row>
     <row r="59" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E59" s="34"/>
       <c r="F59" s="35"/>
-      <c r="G59" s="46" t="s">
+      <c r="G59" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="H59" s="46"/>
-      <c r="I59" s="46"/>
-      <c r="J59" s="46"/>
-      <c r="K59" s="46"/>
+      <c r="H59" s="55"/>
+      <c r="I59" s="55"/>
+      <c r="J59" s="55"/>
+      <c r="K59" s="55"/>
       <c r="L59" s="38"/>
     </row>
     <row r="60" spans="4:12" x14ac:dyDescent="0.3">
@@ -3067,23 +3101,23 @@
       </c>
       <c r="G61" s="39">
         <f>+(G27-$Q15)/$Q15</f>
-        <v>2.5703458523452648E-2</v>
+        <v>-1</v>
       </c>
       <c r="H61" s="39">
         <f t="shared" ref="H61:K61" si="7">+(H27-$Q15)/$Q15</f>
-        <v>2.1368015291893295E-2</v>
+        <v>-1</v>
       </c>
       <c r="I61" s="39">
         <f t="shared" si="7"/>
-        <v>6.8678531395389777E-3</v>
+        <v>-1</v>
       </c>
       <c r="J61" s="39">
         <f t="shared" si="7"/>
-        <v>1.0883048478539001E-2</v>
+        <v>-1</v>
       </c>
       <c r="K61" s="39">
         <f t="shared" si="7"/>
-        <v>1.4984463137405094E-2</v>
+        <v>-1</v>
       </c>
       <c r="L61" s="38"/>
     </row>
@@ -3093,20 +3127,20 @@
         <v>2</v>
       </c>
       <c r="G62" s="39">
-        <f t="shared" ref="G62:K62" si="8">+(G28-$Q16)/$Q16</f>
-        <v>1.2371255744125485E-2</v>
+        <f>+(G28-$Q16)/$Q16</f>
+        <v>1.4262333193606716E-2</v>
       </c>
       <c r="H62" s="39">
-        <f t="shared" si="8"/>
-        <v>1.1401531390679126E-2</v>
+        <f t="shared" ref="H62:K62" si="8">+(H28-$Q16)/$Q16</f>
+        <v>1.3205038018301349E-2</v>
       </c>
       <c r="I62" s="39">
         <f t="shared" si="8"/>
-        <v>1.37748263026804E-2</v>
+        <v>1.2623075253811037E-2</v>
       </c>
       <c r="J62" s="39">
         <f t="shared" si="8"/>
-        <v>1.2810102406492885E-2</v>
+        <v>1.3559442285588547E-2</v>
       </c>
       <c r="K62" s="39">
         <f t="shared" si="8"/>
@@ -3120,24 +3154,24 @@
         <v>0</v>
       </c>
       <c r="G63" s="39">
-        <f t="shared" ref="G63:K63" si="9">+(G29-$Q17)/$Q17</f>
-        <v>-0.11261616498469308</v>
+        <f>+(G29-$Q17)/$Q17</f>
+        <v>-1</v>
       </c>
       <c r="H63" s="39">
-        <f t="shared" si="9"/>
-        <v>-0.19605653748740545</v>
+        <f t="shared" ref="H63:K63" si="9">+(H29-$Q17)/$Q17</f>
+        <v>-1</v>
       </c>
       <c r="I63" s="39">
         <f t="shared" si="9"/>
-        <v>-0.12532902502159451</v>
+        <v>-1</v>
       </c>
       <c r="J63" s="39">
         <f t="shared" si="9"/>
-        <v>-1.6865541137217839E-2</v>
+        <v>-1</v>
       </c>
       <c r="K63" s="39">
         <f t="shared" si="9"/>
-        <v>-5.3577917871420473E-2</v>
+        <v>-1</v>
       </c>
       <c r="L63" s="38"/>
     </row>
@@ -3147,24 +3181,24 @@
         <v>3</v>
       </c>
       <c r="G64" s="39">
-        <f t="shared" ref="G64:K64" si="10">+(G30-$Q18)/$Q18</f>
-        <v>0.3099292638197535</v>
+        <f>+(G30-$Q18)/$Q18</f>
+        <v>-1</v>
       </c>
       <c r="H64" s="39">
-        <f t="shared" si="10"/>
-        <v>0.55923838177254548</v>
+        <f t="shared" ref="H64:K64" si="10">+(H30-$Q18)/$Q18</f>
+        <v>-1</v>
       </c>
       <c r="I64" s="39">
         <f t="shared" si="10"/>
-        <v>0.35429783565880929</v>
+        <v>-1</v>
       </c>
       <c r="J64" s="39">
         <f t="shared" si="10"/>
-        <v>-4.5019310892698033E-2</v>
+        <v>-1</v>
       </c>
       <c r="K64" s="39">
         <f t="shared" si="10"/>
-        <v>0.26556069198069493</v>
+        <v>-1</v>
       </c>
       <c r="L64" s="38"/>
     </row>
@@ -3174,24 +3208,24 @@
         <v>32</v>
       </c>
       <c r="G65" s="39">
-        <f t="shared" ref="G65:K65" si="11">+(G31-$Q19)/$Q19</f>
-        <v>-5.7091583781983257E-2</v>
+        <f>+(G31-$Q19)/$Q19</f>
+        <v>-1</v>
       </c>
       <c r="H65" s="39">
-        <f t="shared" si="11"/>
-        <v>-0.11910047983958334</v>
+        <f t="shared" ref="H65:K65" si="11">+(H31-$Q19)/$Q19</f>
+        <v>-1</v>
       </c>
       <c r="I65" s="39">
         <f t="shared" si="11"/>
-        <v>-6.507978180333325E-2</v>
+        <v>-1</v>
       </c>
       <c r="J65" s="39">
         <f t="shared" si="11"/>
-        <v>-1.9862954289191655E-2</v>
+        <v>-1</v>
       </c>
       <c r="K65" s="39">
         <f t="shared" si="11"/>
-        <v>-7.4236097302333532E-3</v>
+        <v>-1</v>
       </c>
       <c r="L65" s="38"/>
     </row>
@@ -3235,48 +3269,114 @@
       <c r="K69" s="44"/>
       <c r="L69" s="45"/>
     </row>
+    <row r="71" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="G71" t="s">
+        <v>40</v>
+      </c>
+      <c r="H71" t="s">
+        <v>41</v>
+      </c>
+      <c r="I71" t="s">
+        <v>43</v>
+      </c>
+      <c r="J71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="F72" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G72" s="62">
+        <v>0.78537632673401603</v>
+      </c>
+      <c r="H72" s="64">
+        <f>370.970108131567</f>
+        <v>370.97010813156697</v>
+      </c>
+      <c r="I72" s="24">
+        <v>1.7555187933877524E-3</v>
+      </c>
+      <c r="J72" s="24">
+        <v>1.6010771971560166E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="F73" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="G73" s="62">
+        <v>0.78402478355865801</v>
+      </c>
+      <c r="H73" s="63">
+        <v>382.23689426581001</v>
+      </c>
+      <c r="I73" s="24">
+        <v>3.1611681961711006E-5</v>
+      </c>
+      <c r="J73" s="24">
+        <v>1.4262333193606716E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="F74" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="G74" s="62">
+        <v>0.78348144888675997</v>
+      </c>
+      <c r="H74" s="64">
+        <v>419.084818784395</v>
+      </c>
+      <c r="I74" s="24">
+        <v>-6.6141723627558956E-4</v>
+      </c>
+      <c r="J74" s="24">
+        <v>1.3559442285588547E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="F75" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" s="62">
+        <v>0.78320749438814696</v>
+      </c>
+      <c r="H75" s="64">
+        <v>409.63159538507398</v>
+      </c>
+      <c r="I75" s="24">
+        <v>-1.0108489947105448E-3</v>
+      </c>
+      <c r="J75" s="24">
+        <v>1.3205038018301349E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="F76" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G76" s="62">
+        <v>0.78275763717119595</v>
+      </c>
+      <c r="H76" s="64">
+        <v>389.84634193181898</v>
+      </c>
+      <c r="I76" s="24">
+        <v>-1.5846464653113236E-3</v>
+      </c>
+      <c r="J76" s="24">
+        <v>1.2623075253811037E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="F77" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O31:P34">
-    <sortCondition descending="1" ref="P31:P34"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F72:J76">
+    <sortCondition descending="1" ref="G72:G76"/>
   </sortState>
   <mergeCells count="53">
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="I53:I54"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="I55:I56"/>
-    <mergeCell ref="J55:J56"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:G44"/>
-    <mergeCell ref="H43:H44"/>
     <mergeCell ref="G34:K34"/>
     <mergeCell ref="G59:K59"/>
     <mergeCell ref="E3:H3"/>
@@ -3293,6 +3393,43 @@
     <mergeCell ref="J49:J50"/>
     <mergeCell ref="I51:I52"/>
     <mergeCell ref="J51:J52"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="I53:I54"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Agrega ejecucion de trabajo final
</commit_message>
<xml_diff>
--- a/data/Resultados_AG.xlsx
+++ b/data/Resultados_AG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasal\Google Drive\EAFIT\Ciencia de Datos y Analitica\03 Tercer Semestre\Metodos Heuristicos para Optimizacion\metodos-heuristicos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD21EC6B-A900-4A58-A179-7D60A6733380}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B201E66E-A558-48FD-BD47-65831BE82584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B1250CC-1120-467C-8907-0AF514310821}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6B1250CC-1120-467C-8907-0AF514310821}"/>
   </bookViews>
   <sheets>
     <sheet name="AG" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="49">
   <si>
     <t>Precision</t>
   </si>
@@ -165,6 +165,21 @@
   </si>
   <si>
     <t>DP mejor solución</t>
+  </si>
+  <si>
+    <t>DP peor solución</t>
+  </si>
+  <si>
+    <t>Modelo 1 - NAP</t>
+  </si>
+  <si>
+    <t>BE - NAP</t>
+  </si>
+  <si>
+    <t>LS-RB1 - NAP</t>
+  </si>
+  <si>
+    <t>LS-RB1 &amp; BE- NAP</t>
   </si>
 </sst>
 </file>
@@ -174,8 +189,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -516,30 +531,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -555,13 +550,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1802,10 +1817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0DA66-6DF4-4FA4-8913-44EB5171D2D4}">
-  <dimension ref="D2:S77"/>
+  <dimension ref="D2:S86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D39" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+    <sheetView tabSelected="1" topLeftCell="D62" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82:F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1823,25 +1838,25 @@
   <sheetData>
     <row r="2" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="56" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="58"/>
-      <c r="O3" s="56" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="54"/>
+      <c r="O3" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="58"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="54"/>
     </row>
     <row r="4" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D4" s="4" t="s">
@@ -2110,23 +2125,23 @@
     </row>
     <row r="12" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59" t="s">
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="O13" s="56" t="s">
+      <c r="I13" s="55"/>
+      <c r="J13" s="55"/>
+      <c r="O13" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="57"/>
-      <c r="S13" s="58"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="53"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="54"/>
     </row>
     <row r="14" spans="4:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
@@ -2540,22 +2555,22 @@
     <row r="32" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D32" s="1"/>
       <c r="E32" s="34"/>
-      <c r="F32" s="61" t="s">
+      <c r="F32" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="G32" s="63">
+      <c r="G32" s="49">
         <v>382.23689426581001</v>
       </c>
-      <c r="H32" s="64">
+      <c r="H32" s="50">
         <v>409.63159538507398</v>
       </c>
-      <c r="I32" s="64">
+      <c r="I32" s="50">
         <v>389.84634193181898</v>
       </c>
-      <c r="J32" s="64">
+      <c r="J32" s="50">
         <v>419.084818784395</v>
       </c>
-      <c r="K32" s="64">
+      <c r="K32" s="50">
         <f>370.970108131567</f>
         <v>370.97010813156697</v>
       </c>
@@ -2588,13 +2603,13 @@
       <c r="D34" s="1"/>
       <c r="E34" s="34"/>
       <c r="F34" s="35"/>
-      <c r="G34" s="55" t="s">
+      <c r="G34" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H34" s="55"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="51"/>
       <c r="L34" s="38"/>
       <c r="O34" t="s">
         <v>36</v>
@@ -2787,40 +2802,40 @@
       <c r="L42" s="38"/>
     </row>
     <row r="43" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="53"/>
-      <c r="E43" s="51" t="s">
+      <c r="D43" s="56"/>
+      <c r="E43" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="52"/>
-      <c r="G43" s="52"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="52" t="s">
+      <c r="F43" s="59"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="K43" s="52"/>
+      <c r="K43" s="59"/>
       <c r="L43" s="60"/>
-      <c r="M43" s="53"/>
-      <c r="N43" s="48"/>
+      <c r="M43" s="56"/>
+      <c r="N43" s="57"/>
     </row>
     <row r="44" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="53"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="52"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="58"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
       <c r="L44" s="60"/>
-      <c r="M44" s="53"/>
-      <c r="N44" s="48"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="57"/>
     </row>
     <row r="45" spans="4:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="48" t="s">
+      <c r="D45" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="51" t="s">
+      <c r="E45" s="62" t="s">
         <v>19</v>
       </c>
       <c r="F45" s="40" t="s">
@@ -2829,7 +2844,7 @@
       <c r="G45" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="H45" s="52" t="s">
+      <c r="H45" s="59" t="s">
         <v>19</v>
       </c>
       <c r="I45" s="40" t="s">
@@ -2842,26 +2857,26 @@
       <c r="L45" s="38"/>
     </row>
     <row r="46" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="48"/>
-      <c r="E46" s="51"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="62"/>
       <c r="F46" s="41"/>
       <c r="G46" s="41"/>
-      <c r="H46" s="52"/>
+      <c r="H46" s="59"/>
       <c r="I46" s="41"/>
       <c r="J46" s="41"/>
       <c r="K46" s="35"/>
       <c r="L46" s="38"/>
     </row>
     <row r="47" spans="4:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="48"/>
-      <c r="E47" s="51"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="62"/>
       <c r="F47" s="40" t="s">
         <v>21</v>
       </c>
       <c r="G47" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="H47" s="52"/>
+      <c r="H47" s="59"/>
       <c r="I47" s="40" t="s">
         <v>21</v>
       </c>
@@ -2872,206 +2887,206 @@
       <c r="L47" s="38"/>
     </row>
     <row r="48" spans="4:16" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="48"/>
-      <c r="E48" s="51"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="62"/>
       <c r="F48" s="42"/>
       <c r="G48" s="42"/>
-      <c r="H48" s="52"/>
+      <c r="H48" s="59"/>
       <c r="I48" s="42"/>
       <c r="J48" s="42"/>
       <c r="K48" s="35"/>
       <c r="L48" s="38"/>
     </row>
     <row r="49" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="48" t="s">
+      <c r="D49" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="E49" s="49">
+      <c r="E49" s="63">
         <v>0.06</v>
       </c>
-      <c r="F49" s="47">
+      <c r="F49" s="61">
         <v>-1.83E-2</v>
       </c>
-      <c r="G49" s="47">
+      <c r="G49" s="61">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="H49" s="50">
+      <c r="H49" s="64">
         <v>0.06</v>
       </c>
-      <c r="I49" s="47">
+      <c r="I49" s="61">
         <v>-1.0999999999999999E-2</v>
       </c>
-      <c r="J49" s="47">
+      <c r="J49" s="61">
         <v>2.2499999999999999E-2</v>
       </c>
       <c r="K49" s="35"/>
       <c r="L49" s="38"/>
     </row>
     <row r="50" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="48"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="47"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="64"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="61"/>
       <c r="K50" s="35"/>
       <c r="L50" s="38"/>
     </row>
     <row r="51" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="48" t="s">
+      <c r="D51" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E51" s="49">
+      <c r="E51" s="63">
         <v>0.78500000000000003</v>
       </c>
-      <c r="F51" s="47">
+      <c r="F51" s="61">
         <v>1.8E-3</v>
       </c>
-      <c r="G51" s="47">
+      <c r="G51" s="61">
         <v>1.6E-2</v>
       </c>
-      <c r="H51" s="50">
+      <c r="H51" s="64">
         <v>0.78400000000000003</v>
       </c>
-      <c r="I51" s="47">
+      <c r="I51" s="61">
         <v>-1E-4</v>
       </c>
-      <c r="J51" s="47">
+      <c r="J51" s="61">
         <v>1.41E-2</v>
       </c>
       <c r="K51" s="35"/>
       <c r="L51" s="38"/>
     </row>
     <row r="52" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="48"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="50"/>
-      <c r="I52" s="47"/>
-      <c r="J52" s="47"/>
+      <c r="D52" s="57"/>
+      <c r="E52" s="63"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="61"/>
+      <c r="H52" s="64"/>
+      <c r="I52" s="61"/>
+      <c r="J52" s="61"/>
       <c r="K52" s="35"/>
       <c r="L52" s="38"/>
     </row>
     <row r="53" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="48" t="s">
+      <c r="D53" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E53" s="49">
+      <c r="E53" s="63">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="F53" s="47">
+      <c r="F53" s="61">
         <v>4.6800000000000001E-2</v>
       </c>
-      <c r="G53" s="47">
+      <c r="G53" s="61">
         <v>-5.3600000000000002E-2</v>
       </c>
-      <c r="H53" s="50">
+      <c r="H53" s="64">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="I53" s="47">
+      <c r="I53" s="61">
         <v>-3.7400000000000003E-2</v>
       </c>
-      <c r="J53" s="47">
+      <c r="J53" s="61">
         <v>-0.12970000000000001</v>
       </c>
       <c r="K53" s="35"/>
       <c r="L53" s="38"/>
     </row>
     <row r="54" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="48"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="47"/>
-      <c r="G54" s="47"/>
-      <c r="H54" s="50"/>
-      <c r="I54" s="47"/>
-      <c r="J54" s="47"/>
+      <c r="D54" s="57"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="61"/>
+      <c r="H54" s="64"/>
+      <c r="I54" s="61"/>
+      <c r="J54" s="61"/>
       <c r="K54" s="35"/>
       <c r="L54" s="38"/>
     </row>
     <row r="55" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="48" t="s">
+      <c r="D55" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="49">
+      <c r="E55" s="63">
         <v>0.432</v>
       </c>
-      <c r="F55" s="47">
+      <c r="F55" s="61">
         <v>-4.7300000000000002E-2</v>
       </c>
-      <c r="G55" s="47">
+      <c r="G55" s="61">
         <v>0.2656</v>
       </c>
-      <c r="H55" s="50">
+      <c r="H55" s="64">
         <v>0.496</v>
       </c>
-      <c r="I55" s="47">
+      <c r="I55" s="61">
         <v>9.4200000000000006E-2</v>
       </c>
-      <c r="J55" s="47">
+      <c r="J55" s="61">
         <v>0.4536</v>
       </c>
       <c r="K55" s="35"/>
       <c r="L55" s="38"/>
     </row>
     <row r="56" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="48"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="50"/>
-      <c r="I56" s="47"/>
-      <c r="J56" s="47"/>
+      <c r="D56" s="57"/>
+      <c r="E56" s="63"/>
+      <c r="F56" s="61"/>
+      <c r="G56" s="61"/>
+      <c r="H56" s="64"/>
+      <c r="I56" s="61"/>
+      <c r="J56" s="61"/>
       <c r="K56" s="35"/>
       <c r="L56" s="38"/>
     </row>
     <row r="57" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="48" t="s">
+      <c r="D57" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="E57" s="49">
+      <c r="E57" s="63">
         <v>0.11899999999999999</v>
       </c>
-      <c r="F57" s="47">
+      <c r="F57" s="61">
         <v>3.5700000000000003E-2</v>
       </c>
-      <c r="G57" s="47">
+      <c r="G57" s="61">
         <v>-7.4000000000000003E-3</v>
       </c>
-      <c r="H57" s="50">
+      <c r="H57" s="64">
         <v>0.113</v>
       </c>
-      <c r="I57" s="47">
+      <c r="I57" s="61">
         <v>-2.06E-2</v>
       </c>
-      <c r="J57" s="47">
+      <c r="J57" s="61">
         <v>-6.1400000000000003E-2</v>
       </c>
       <c r="K57" s="35"/>
       <c r="L57" s="38"/>
     </row>
     <row r="58" spans="4:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="48"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="50"/>
-      <c r="I58" s="47"/>
-      <c r="J58" s="47"/>
+      <c r="D58" s="57"/>
+      <c r="E58" s="63"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="64"/>
+      <c r="I58" s="61"/>
+      <c r="J58" s="61"/>
       <c r="K58" s="35"/>
       <c r="L58" s="38"/>
     </row>
     <row r="59" spans="4:12" x14ac:dyDescent="0.3">
       <c r="E59" s="34"/>
       <c r="F59" s="35"/>
-      <c r="G59" s="55" t="s">
+      <c r="G59" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="H59" s="55"/>
-      <c r="I59" s="55"/>
-      <c r="J59" s="55"/>
-      <c r="K59" s="55"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="51"/>
+      <c r="K59" s="51"/>
       <c r="L59" s="38"/>
     </row>
     <row r="60" spans="4:12" x14ac:dyDescent="0.3">
@@ -3287,10 +3302,10 @@
       <c r="F72" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="G72" s="62">
+      <c r="G72" s="48">
         <v>0.78537632673401603</v>
       </c>
-      <c r="H72" s="64">
+      <c r="H72" s="50">
         <f>370.970108131567</f>
         <v>370.97010813156697</v>
       </c>
@@ -3305,10 +3320,10 @@
       <c r="F73" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="G73" s="62">
+      <c r="G73" s="48">
         <v>0.78402478355865801</v>
       </c>
-      <c r="H73" s="63">
+      <c r="H73" s="49">
         <v>382.23689426581001</v>
       </c>
       <c r="I73" s="24">
@@ -3322,10 +3337,10 @@
       <c r="F74" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G74" s="62">
+      <c r="G74" s="48">
         <v>0.78348144888675997</v>
       </c>
-      <c r="H74" s="64">
+      <c r="H74" s="50">
         <v>419.084818784395</v>
       </c>
       <c r="I74" s="24">
@@ -3339,10 +3354,10 @@
       <c r="F75" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="G75" s="62">
+      <c r="G75" s="48">
         <v>0.78320749438814696</v>
       </c>
-      <c r="H75" s="64">
+      <c r="H75" s="50">
         <v>409.63159538507398</v>
       </c>
       <c r="I75" s="24">
@@ -3356,10 +3371,10 @@
       <c r="F76" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G76" s="62">
+      <c r="G76" s="48">
         <v>0.78275763717119595</v>
       </c>
-      <c r="H76" s="64">
+      <c r="H76" s="50">
         <v>389.84634193181898</v>
       </c>
       <c r="I76" s="24">
@@ -3371,12 +3386,159 @@
     </row>
     <row r="77" spans="5:12" x14ac:dyDescent="0.3">
       <c r="F77" s="1"/>
+    </row>
+    <row r="81" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="G81" t="s">
+        <v>40</v>
+      </c>
+      <c r="H81" t="s">
+        <v>41</v>
+      </c>
+      <c r="I81" t="s">
+        <v>43</v>
+      </c>
+      <c r="J81" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F82" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G82" s="48">
+        <v>0.78537632673401603</v>
+      </c>
+      <c r="H82" s="50">
+        <f>370.970108131567</f>
+        <v>370.97010813156697</v>
+      </c>
+      <c r="I82" s="24">
+        <f>(G82-$Q$6)/$Q$6</f>
+        <v>1.7555187933877524E-3</v>
+      </c>
+      <c r="J82" s="24">
+        <f>(G82-$Q$16)/$Q$16</f>
+        <v>1.6010771971560166E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F83" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G83" s="48">
+        <v>0.78300480612999201</v>
+      </c>
+      <c r="H83" s="50">
+        <v>321.52</v>
+      </c>
+      <c r="I83" s="24">
+        <f t="shared" ref="I83:I86" si="12">(G83-$Q$6)/$Q$6</f>
+        <v>-1.2693799362347134E-3</v>
+      </c>
+      <c r="J83" s="24">
+        <f t="shared" ref="J83:J86" si="13">(G83-$Q$16)/$Q$16</f>
+        <v>1.2942828111244494E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F84" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="G84" s="48">
+        <v>0.78270945622013199</v>
+      </c>
+      <c r="H84" s="50">
+        <v>372.08</v>
+      </c>
+      <c r="I84" s="24">
+        <f t="shared" si="12"/>
+        <v>-1.6461017600357605E-3</v>
+      </c>
+      <c r="J84" s="24">
+        <f t="shared" si="13"/>
+        <v>1.2560745433547184E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F85" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="G85" s="48">
+        <v>0.78324405985493994</v>
+      </c>
+      <c r="H85" s="50">
+        <v>294.88</v>
+      </c>
+      <c r="I85" s="24">
+        <f t="shared" si="12"/>
+        <v>-9.6420936869908867E-4</v>
+      </c>
+      <c r="J85" s="24">
+        <f t="shared" si="13"/>
+        <v>1.325234133886148E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F86" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="G86" s="48">
+        <v>0.78261697909535199</v>
+      </c>
+      <c r="H86" s="50">
+        <v>226.67</v>
+      </c>
+      <c r="I86" s="24">
+        <f t="shared" si="12"/>
+        <v>-1.7640572763367801E-3</v>
+      </c>
+      <c r="J86" s="24">
+        <f t="shared" si="13"/>
+        <v>1.2441111378204365E-2</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F72:J76">
     <sortCondition descending="1" ref="G72:G76"/>
   </sortState>
   <mergeCells count="53">
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="I53:I54"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:G44"/>
+    <mergeCell ref="H43:H44"/>
     <mergeCell ref="G34:K34"/>
     <mergeCell ref="G59:K59"/>
     <mergeCell ref="E3:H3"/>
@@ -3393,46 +3555,9 @@
     <mergeCell ref="J49:J50"/>
     <mergeCell ref="I51:I52"/>
     <mergeCell ref="J51:J52"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="I53:I54"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="I55:I56"/>
-    <mergeCell ref="J55:J56"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="H57:H58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>